<commit_message>
Updated Summer Series points
</commit_message>
<xml_diff>
--- a/points_csv.xlsx
+++ b/points_csv.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\Desktop\Projects\VIKA\2022_Website\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8468710F-CC23-4832-AD1E-F8EED8D760A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BD8FA437-E160-442F-B222-4B232E4527A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" activeTab="1" xr2:uid="{F04811E9-38A3-4B99-BDED-515010F258AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" activeTab="2" xr2:uid="{F04811E9-38A3-4B99-BDED-515010F258AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Distribution" sheetId="1" r:id="rId1"/>
     <sheet name="points_csv" sheetId="2" r:id="rId2"/>
+    <sheet name="2022_summer_series_positions" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">points_csv!$A$72:$F$101</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="181">
   <si>
     <t>offset</t>
   </si>
@@ -407,16 +408,196 @@
   </si>
   <si>
     <t>Tony Church</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>4 Cycle - Open</t>
+  </si>
+  <si>
+    <t>Hazen Vertado</t>
+  </si>
+  <si>
+    <t>Janel church</t>
+  </si>
+  <si>
+    <t>Jordon Wilson</t>
+  </si>
+  <si>
+    <t>Kevin .Roberts</t>
+  </si>
+  <si>
+    <t>Andres Navarrete</t>
+  </si>
+  <si>
+    <t>Jr 1 Briggs LO206</t>
+  </si>
+  <si>
+    <t>Archer Eror</t>
+  </si>
+  <si>
+    <t>Jr 2 Briggs LO206</t>
+  </si>
+  <si>
+    <t>Caleb E</t>
+  </si>
+  <si>
+    <t>Kayden Martens</t>
+  </si>
+  <si>
+    <t>Liam Cormier</t>
+  </si>
+  <si>
+    <t>Sr Briggs LO206</t>
+  </si>
+  <si>
+    <t>Dave Cormier</t>
+  </si>
+  <si>
+    <t>Kyle Matthews</t>
+  </si>
+  <si>
+    <t>Meagan Hastings</t>
+  </si>
+  <si>
+    <t>Todd  Martin</t>
+  </si>
+  <si>
+    <t>Wes Roberts</t>
+  </si>
+  <si>
+    <t>TaG Cadet</t>
+  </si>
+  <si>
+    <t>Madden Breckwoldt</t>
+  </si>
+  <si>
+    <t>Mason Bemister</t>
+  </si>
+  <si>
+    <t>Tag Masters</t>
+  </si>
+  <si>
+    <t>Alan Zaalberg</t>
+  </si>
+  <si>
+    <t>Jamie Coles</t>
+  </si>
+  <si>
+    <t>John Almond</t>
+  </si>
+  <si>
+    <t>Josiah Reaume</t>
+  </si>
+  <si>
+    <t>Michael Chalk</t>
+  </si>
+  <si>
+    <t>Wouter Bouman</t>
+  </si>
+  <si>
+    <t>Boris Jurcic</t>
+  </si>
+  <si>
+    <t>Doug Hopwood</t>
+  </si>
+  <si>
+    <t>JONATHAN REAUME</t>
+  </si>
+  <si>
+    <t>Kristian Dinkov</t>
+  </si>
+  <si>
+    <t>Matthew Bahen</t>
+  </si>
+  <si>
+    <t>Scott Hoadley</t>
+  </si>
+  <si>
+    <t>Sean Michelljones</t>
+  </si>
+  <si>
+    <t>Steven Healey</t>
+  </si>
+  <si>
+    <t>Tayler Rand</t>
+  </si>
+  <si>
+    <t>Race 1 - Qualifying</t>
+  </si>
+  <si>
+    <t>Race 1 - Pre-final</t>
+  </si>
+  <si>
+    <t>Race 1 - Final</t>
+  </si>
+  <si>
+    <t>Race 2 - Qualifying</t>
+  </si>
+  <si>
+    <t>Race 2 - Pre-final</t>
+  </si>
+  <si>
+    <t>Race 2 - Final</t>
+  </si>
+  <si>
+    <t>DQ</t>
+  </si>
+  <si>
+    <t>Kade George</t>
+  </si>
+  <si>
+    <t>Joao Farinha</t>
+  </si>
+  <si>
+    <t>Alex Jay</t>
+  </si>
+  <si>
+    <t>Ben Harris</t>
+  </si>
+  <si>
+    <t>Aaron Thomas</t>
+  </si>
+  <si>
+    <t>Kellen Ritter</t>
+  </si>
+  <si>
+    <t>Matthew De Groot</t>
+  </si>
+  <si>
+    <t>Jake Tchida</t>
+  </si>
+  <si>
+    <t>Tim Tchida</t>
+  </si>
+  <si>
+    <t>Gerry Rang</t>
+  </si>
+  <si>
+    <t>Jer Bird</t>
+  </si>
+  <si>
+    <t>Isaac Finer</t>
+  </si>
+  <si>
+    <t>Bill Karas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5172,6 +5353,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>600839</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>144038</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDFB8B9F-E67B-4054-9B72-481388C1C352}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16992600" y="571500"/>
+          <a:ext cx="5477639" cy="8335538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5968,7 +6198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333DEC3A-8273-4877-A171-E37DE3F80C8C}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I125" sqref="I125"/>
     </sheetView>
   </sheetViews>
@@ -6015,7 +6245,7 @@
         <v>550</v>
       </c>
       <c r="F2">
-        <f>SUM(C2,D2,E2)</f>
+        <f t="shared" ref="F2:F30" si="0">SUM(C2,D2,E2)</f>
         <v>1585</v>
       </c>
     </row>
@@ -6036,7 +6266,7 @@
         <v>510</v>
       </c>
       <c r="F3">
-        <f>SUM(C3,D3,E3)</f>
+        <f t="shared" si="0"/>
         <v>1445</v>
       </c>
     </row>
@@ -6057,7 +6287,7 @@
         <v>420</v>
       </c>
       <c r="F4">
-        <f>SUM(C4,D4,E4)</f>
+        <f t="shared" si="0"/>
         <v>1325</v>
       </c>
     </row>
@@ -6078,7 +6308,7 @@
         <v>410</v>
       </c>
       <c r="F5">
-        <f>SUM(C5,D5,E5)</f>
+        <f t="shared" si="0"/>
         <v>1270</v>
       </c>
     </row>
@@ -6099,7 +6329,7 @@
         <v>600</v>
       </c>
       <c r="F6">
-        <f>SUM(C6,D6,E6)</f>
+        <f t="shared" si="0"/>
         <v>1150</v>
       </c>
     </row>
@@ -6120,7 +6350,7 @@
         <v>360</v>
       </c>
       <c r="F7">
-        <f>SUM(C7,D7,E7)</f>
+        <f t="shared" si="0"/>
         <v>1140</v>
       </c>
     </row>
@@ -6141,7 +6371,7 @@
         <v>340</v>
       </c>
       <c r="F8">
-        <f>SUM(C8,D8,E8)</f>
+        <f t="shared" si="0"/>
         <v>1135</v>
       </c>
     </row>
@@ -6162,7 +6392,7 @@
         <v>485</v>
       </c>
       <c r="F9">
-        <f>SUM(C9,D9,E9)</f>
+        <f t="shared" si="0"/>
         <v>995</v>
       </c>
     </row>
@@ -6183,7 +6413,7 @@
         <v>315</v>
       </c>
       <c r="F10">
-        <f>SUM(C10,D10,E10)</f>
+        <f t="shared" si="0"/>
         <v>915</v>
       </c>
     </row>
@@ -6204,7 +6434,7 @@
         <v>450</v>
       </c>
       <c r="F11">
-        <f>SUM(C11,D11,E11)</f>
+        <f t="shared" si="0"/>
         <v>900</v>
       </c>
     </row>
@@ -6225,7 +6455,7 @@
         <v>390</v>
       </c>
       <c r="F12">
-        <f>SUM(C12,D12,E12)</f>
+        <f t="shared" si="0"/>
         <v>820</v>
       </c>
     </row>
@@ -6246,7 +6476,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <f>SUM(C13,D13,E13)</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
     </row>
@@ -6267,7 +6497,7 @@
         <v>400</v>
       </c>
       <c r="F14">
-        <f>SUM(C14,D14,E14)</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
     </row>
@@ -6288,7 +6518,7 @@
         <v>375</v>
       </c>
       <c r="F15">
-        <f>SUM(C15,D15,E15)</f>
+        <f t="shared" si="0"/>
         <v>785</v>
       </c>
     </row>
@@ -6309,7 +6539,7 @@
         <v>355</v>
       </c>
       <c r="F16">
-        <f>SUM(C16,D16,E16)</f>
+        <f t="shared" si="0"/>
         <v>735</v>
       </c>
     </row>
@@ -6330,7 +6560,7 @@
         <v>320</v>
       </c>
       <c r="F17">
-        <f>SUM(C17,D17,E17)</f>
+        <f t="shared" si="0"/>
         <v>685</v>
       </c>
     </row>
@@ -6351,7 +6581,7 @@
         <v>310</v>
       </c>
       <c r="F18">
-        <f>SUM(C18,D18,E18)</f>
+        <f t="shared" si="0"/>
         <v>650</v>
       </c>
     </row>
@@ -6372,7 +6602,7 @@
         <v>430</v>
       </c>
       <c r="F19">
-        <f>SUM(C19,D19,E19)</f>
+        <f t="shared" si="0"/>
         <v>430</v>
       </c>
     </row>
@@ -6393,7 +6623,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <f>SUM(C20,D20,E20)</f>
+        <f t="shared" si="0"/>
         <v>410</v>
       </c>
     </row>
@@ -6414,7 +6644,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <f>SUM(C21,D21,E21)</f>
+        <f t="shared" si="0"/>
         <v>390</v>
       </c>
     </row>
@@ -6435,7 +6665,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <f>SUM(C22,D22,E22)</f>
+        <f t="shared" si="0"/>
         <v>375</v>
       </c>
     </row>
@@ -6456,7 +6686,7 @@
         <v>370</v>
       </c>
       <c r="F23">
-        <f>SUM(C23,D23,E23)</f>
+        <f t="shared" si="0"/>
         <v>370</v>
       </c>
     </row>
@@ -6477,7 +6707,7 @@
         <v>365</v>
       </c>
       <c r="F24">
-        <f>SUM(C24,D24,E24)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
     </row>
@@ -6498,7 +6728,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <f>SUM(C25,D25,E25)</f>
+        <f t="shared" si="0"/>
         <v>355</v>
       </c>
     </row>
@@ -6519,7 +6749,7 @@
         <v>350</v>
       </c>
       <c r="F26">
-        <f>SUM(C26,D26,E26)</f>
+        <f t="shared" si="0"/>
         <v>350</v>
       </c>
     </row>
@@ -6540,7 +6770,7 @@
         <v>345</v>
       </c>
       <c r="F27">
-        <f>SUM(C27,D27,E27)</f>
+        <f t="shared" si="0"/>
         <v>345</v>
       </c>
     </row>
@@ -6561,7 +6791,7 @@
         <v>335</v>
       </c>
       <c r="F28">
-        <f>SUM(C28,D28,E28)</f>
+        <f t="shared" si="0"/>
         <v>335</v>
       </c>
     </row>
@@ -6582,7 +6812,7 @@
         <v>330</v>
       </c>
       <c r="F29">
-        <f>SUM(C29,D29,E29)</f>
+        <f t="shared" si="0"/>
         <v>330</v>
       </c>
     </row>
@@ -6603,7 +6833,7 @@
         <v>325</v>
       </c>
       <c r="F30">
-        <f>SUM(C30,D30,E30)</f>
+        <f t="shared" si="0"/>
         <v>325</v>
       </c>
     </row>
@@ -6624,7 +6854,7 @@
         <v>550</v>
       </c>
       <c r="F34">
-        <f>SUM(C34,D34,E34)</f>
+        <f t="shared" ref="F34:F60" si="1">SUM(C34,D34,E34)</f>
         <v>1545</v>
       </c>
     </row>
@@ -6645,7 +6875,7 @@
         <v>600</v>
       </c>
       <c r="F35">
-        <f>SUM(C35,D35,E35)</f>
+        <f t="shared" si="1"/>
         <v>1520</v>
       </c>
     </row>
@@ -6666,7 +6896,7 @@
         <v>510</v>
       </c>
       <c r="F36">
-        <f>SUM(C36,D36,E36)</f>
+        <f t="shared" si="1"/>
         <v>1415</v>
       </c>
     </row>
@@ -6687,7 +6917,7 @@
         <v>420</v>
       </c>
       <c r="F37">
-        <f>SUM(C37,D37,E37)</f>
+        <f t="shared" si="1"/>
         <v>1240</v>
       </c>
     </row>
@@ -6708,7 +6938,7 @@
         <v>430</v>
       </c>
       <c r="F38">
-        <f>SUM(C38,D38,E38)</f>
+        <f t="shared" si="1"/>
         <v>1190</v>
       </c>
     </row>
@@ -6729,7 +6959,7 @@
         <v>365</v>
       </c>
       <c r="F39">
-        <f>SUM(C39,D39,E39)</f>
+        <f t="shared" si="1"/>
         <v>1185</v>
       </c>
     </row>
@@ -6750,7 +6980,7 @@
         <v>410</v>
       </c>
       <c r="F40">
-        <f>SUM(C40,D40,E40)</f>
+        <f t="shared" si="1"/>
         <v>1185</v>
       </c>
     </row>
@@ -6771,7 +7001,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <f>SUM(C41,D41,E41)</f>
+        <f t="shared" si="1"/>
         <v>960</v>
       </c>
     </row>
@@ -6792,7 +7022,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <f>SUM(C42,D42,E42)</f>
+        <f t="shared" si="1"/>
         <v>825</v>
       </c>
     </row>
@@ -6813,7 +7043,7 @@
         <v>390</v>
       </c>
       <c r="F43">
-        <f>SUM(C43,D43,E43)</f>
+        <f t="shared" si="1"/>
         <v>780</v>
       </c>
     </row>
@@ -6834,7 +7064,7 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <f>SUM(C44,D44,E44)</f>
+        <f t="shared" si="1"/>
         <v>770</v>
       </c>
     </row>
@@ -6855,7 +7085,7 @@
         <v>375</v>
       </c>
       <c r="F45">
-        <f>SUM(C45,D45,E45)</f>
+        <f t="shared" si="1"/>
         <v>730</v>
       </c>
     </row>
@@ -6876,7 +7106,7 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <f>SUM(C46,D46,E46)</f>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
     </row>
@@ -6897,7 +7127,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <f>SUM(C47,D47,E47)</f>
+        <f t="shared" si="1"/>
         <v>550</v>
       </c>
     </row>
@@ -6918,7 +7148,7 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <f>SUM(C48,D48,E48)</f>
+        <f t="shared" si="1"/>
         <v>510</v>
       </c>
     </row>
@@ -6939,7 +7169,7 @@
         <v>485</v>
       </c>
       <c r="F49">
-        <f>SUM(C49,D49,E49)</f>
+        <f t="shared" si="1"/>
         <v>485</v>
       </c>
     </row>
@@ -6960,7 +7190,7 @@
         <v>450</v>
       </c>
       <c r="F50">
-        <f>SUM(C50,D50,E50)</f>
+        <f t="shared" si="1"/>
         <v>450</v>
       </c>
     </row>
@@ -6981,7 +7211,7 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <f>SUM(C51,D51,E51)</f>
+        <f t="shared" si="1"/>
         <v>430</v>
       </c>
     </row>
@@ -7002,7 +7232,7 @@
         <v>0</v>
       </c>
       <c r="F52">
-        <f>SUM(C52,D52,E52)</f>
+        <f t="shared" si="1"/>
         <v>410</v>
       </c>
     </row>
@@ -7023,7 +7253,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <f>SUM(C53,D53,E53)</f>
+        <f t="shared" si="1"/>
         <v>410</v>
       </c>
     </row>
@@ -7044,7 +7274,7 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <f>SUM(C54,D54,E54)</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
     </row>
@@ -7065,7 +7295,7 @@
         <v>400</v>
       </c>
       <c r="F55">
-        <f>SUM(C55,D55,E55)</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
     </row>
@@ -7086,7 +7316,7 @@
         <v>370</v>
       </c>
       <c r="F56">
-        <f>SUM(C56,D56,E56)</f>
+        <f t="shared" si="1"/>
         <v>370</v>
       </c>
     </row>
@@ -7107,7 +7337,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <f>SUM(C57,D57,E57)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
     </row>
@@ -7128,7 +7358,7 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <f>SUM(C58,D58,E58)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
     </row>
@@ -7149,7 +7379,7 @@
         <v>365</v>
       </c>
       <c r="F59">
-        <f>SUM(C59,D59,E59)</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
     </row>
@@ -7170,7 +7400,7 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <f>SUM(C60,D60,E60)</f>
+        <f t="shared" si="1"/>
         <v>360</v>
       </c>
     </row>
@@ -7191,7 +7421,7 @@
         <v>550</v>
       </c>
       <c r="F63">
-        <f>SUM(C63,D63,E63)</f>
+        <f t="shared" ref="F63:F70" si="2">SUM(C63,D63,E63)</f>
         <v>1485</v>
       </c>
     </row>
@@ -7212,7 +7442,7 @@
         <v>600</v>
       </c>
       <c r="F64">
-        <f>SUM(C64,D64,E64)</f>
+        <f t="shared" si="2"/>
         <v>1200</v>
       </c>
     </row>
@@ -7233,7 +7463,7 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <f>SUM(C65,D65,E65)</f>
+        <f t="shared" si="2"/>
         <v>1060</v>
       </c>
     </row>
@@ -7254,7 +7484,7 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <f>SUM(C66,D66,E66)</f>
+        <f t="shared" si="2"/>
         <v>1060</v>
       </c>
     </row>
@@ -7275,7 +7505,7 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <f>SUM(C67,D67,E67)</f>
+        <f t="shared" si="2"/>
         <v>600</v>
       </c>
     </row>
@@ -7296,7 +7526,7 @@
         <v>510</v>
       </c>
       <c r="F68">
-        <f>SUM(C68,D68,E68)</f>
+        <f t="shared" si="2"/>
         <v>510</v>
       </c>
     </row>
@@ -7317,7 +7547,7 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <f>SUM(C69,D69,E69)</f>
+        <f t="shared" si="2"/>
         <v>485</v>
       </c>
     </row>
@@ -7338,7 +7568,7 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <f>SUM(C70,D70,E70)</f>
+        <f t="shared" si="2"/>
         <v>450</v>
       </c>
     </row>
@@ -7359,7 +7589,7 @@
         <v>430</v>
       </c>
       <c r="F72">
-        <f>SUM(C72,D72,E72)</f>
+        <f t="shared" ref="F72:F101" si="3">SUM(C72,D72,E72)</f>
         <v>1400</v>
       </c>
     </row>
@@ -7380,7 +7610,7 @@
         <v>370</v>
       </c>
       <c r="F73">
-        <f>SUM(C73,D73,E73)</f>
+        <f t="shared" si="3"/>
         <v>1250</v>
       </c>
     </row>
@@ -7401,7 +7631,7 @@
         <v>375</v>
       </c>
       <c r="F74">
-        <f>SUM(C74,D74,E74)</f>
+        <f t="shared" si="3"/>
         <v>1180</v>
       </c>
     </row>
@@ -7422,7 +7652,7 @@
         <v>355</v>
       </c>
       <c r="F75">
-        <f>SUM(C75,D75,E75)</f>
+        <f t="shared" si="3"/>
         <v>1110</v>
       </c>
     </row>
@@ -7443,7 +7673,7 @@
         <v>550</v>
       </c>
       <c r="F76">
-        <f>SUM(C76,D76,E76)</f>
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
     </row>
@@ -7464,7 +7694,7 @@
         <v>485</v>
       </c>
       <c r="F77">
-        <f>SUM(C77,D77,E77)</f>
+        <f t="shared" si="3"/>
         <v>915</v>
       </c>
     </row>
@@ -7485,7 +7715,7 @@
         <v>450</v>
       </c>
       <c r="F78">
-        <f>SUM(C78,D78,E78)</f>
+        <f t="shared" si="3"/>
         <v>870</v>
       </c>
     </row>
@@ -7506,7 +7736,7 @@
         <v>510</v>
       </c>
       <c r="F79">
-        <f>SUM(C79,D79,E79)</f>
+        <f t="shared" si="3"/>
         <v>860</v>
       </c>
     </row>
@@ -7527,7 +7757,7 @@
         <v>345</v>
       </c>
       <c r="F80">
-        <f>SUM(C80,D80,E80)</f>
+        <f t="shared" si="3"/>
         <v>855</v>
       </c>
     </row>
@@ -7548,7 +7778,7 @@
         <v>380</v>
       </c>
       <c r="F81">
-        <f>SUM(C81,D81,E81)</f>
+        <f t="shared" si="3"/>
         <v>830</v>
       </c>
     </row>
@@ -7569,7 +7799,7 @@
         <v>400</v>
       </c>
       <c r="F82">
-        <f>SUM(C82,D82,E82)</f>
+        <f t="shared" si="3"/>
         <v>790</v>
       </c>
     </row>
@@ -7590,7 +7820,7 @@
         <v>0</v>
       </c>
       <c r="F83">
-        <f>SUM(C83,D83,E83)</f>
+        <f t="shared" si="3"/>
         <v>600</v>
       </c>
     </row>
@@ -7611,7 +7841,7 @@
         <v>0</v>
       </c>
       <c r="F84">
-        <f>SUM(C84,D84,E84)</f>
+        <f t="shared" si="3"/>
         <v>600</v>
       </c>
     </row>
@@ -7632,7 +7862,7 @@
         <v>600</v>
       </c>
       <c r="F85">
-        <f>SUM(C85,D85,E85)</f>
+        <f t="shared" si="3"/>
         <v>600</v>
       </c>
     </row>
@@ -7653,7 +7883,7 @@
         <v>0</v>
       </c>
       <c r="F86">
-        <f>SUM(C86,D86,E86)</f>
+        <f t="shared" si="3"/>
         <v>550</v>
       </c>
     </row>
@@ -7674,7 +7904,7 @@
         <v>0</v>
       </c>
       <c r="F87">
-        <f>SUM(C87,D87,E87)</f>
+        <f t="shared" si="3"/>
         <v>450</v>
       </c>
     </row>
@@ -7695,7 +7925,7 @@
         <v>0</v>
       </c>
       <c r="F88">
-        <f>SUM(C88,D88,E88)</f>
+        <f t="shared" si="3"/>
         <v>420</v>
       </c>
     </row>
@@ -7716,7 +7946,7 @@
         <v>420</v>
       </c>
       <c r="F89">
-        <f>SUM(C89,D89,E89)</f>
+        <f t="shared" si="3"/>
         <v>420</v>
       </c>
     </row>
@@ -7737,7 +7967,7 @@
         <v>0</v>
       </c>
       <c r="F90">
-        <f>SUM(C90,D90,E90)</f>
+        <f t="shared" si="3"/>
         <v>410</v>
       </c>
     </row>
@@ -7758,7 +7988,7 @@
         <v>410</v>
       </c>
       <c r="F91">
-        <f>SUM(C91,D91,E91)</f>
+        <f t="shared" si="3"/>
         <v>410</v>
       </c>
     </row>
@@ -7779,7 +8009,7 @@
         <v>0</v>
       </c>
       <c r="F92">
-        <f>SUM(C92,D92,E92)</f>
+        <f t="shared" si="3"/>
         <v>400</v>
       </c>
     </row>
@@ -7800,7 +8030,7 @@
         <v>0</v>
       </c>
       <c r="F93">
-        <f>SUM(C93,D93,E93)</f>
+        <f t="shared" si="3"/>
         <v>400</v>
       </c>
     </row>
@@ -7821,7 +8051,7 @@
         <v>390</v>
       </c>
       <c r="F94">
-        <f>SUM(C94,D94,E94)</f>
+        <f t="shared" si="3"/>
         <v>390</v>
       </c>
     </row>
@@ -7842,7 +8072,7 @@
         <v>0</v>
       </c>
       <c r="F95">
-        <f>SUM(C95,D95,E95)</f>
+        <f t="shared" si="3"/>
         <v>380</v>
       </c>
     </row>
@@ -7863,7 +8093,7 @@
         <v>0</v>
       </c>
       <c r="F96">
-        <f>SUM(C96,D96,E96)</f>
+        <f t="shared" si="3"/>
         <v>375</v>
       </c>
     </row>
@@ -7884,7 +8114,7 @@
         <v>365</v>
       </c>
       <c r="F97">
-        <f>SUM(C97,D97,E97)</f>
+        <f t="shared" si="3"/>
         <v>365</v>
       </c>
     </row>
@@ -7905,7 +8135,7 @@
         <v>0</v>
       </c>
       <c r="F98">
-        <f>SUM(C98,D98,E98)</f>
+        <f t="shared" si="3"/>
         <v>360</v>
       </c>
     </row>
@@ -7926,7 +8156,7 @@
         <v>360</v>
       </c>
       <c r="F99">
-        <f>SUM(C99,D99,E99)</f>
+        <f t="shared" si="3"/>
         <v>360</v>
       </c>
     </row>
@@ -7947,7 +8177,7 @@
         <v>0</v>
       </c>
       <c r="F100">
-        <f>SUM(C100,D100,E100)</f>
+        <f t="shared" si="3"/>
         <v>355</v>
       </c>
     </row>
@@ -7968,7 +8198,7 @@
         <v>350</v>
       </c>
       <c r="F101">
-        <f>SUM(C101,D101,E101)</f>
+        <f t="shared" si="3"/>
         <v>350</v>
       </c>
     </row>
@@ -7989,7 +8219,7 @@
         <v>600</v>
       </c>
       <c r="F104">
-        <f>SUM(C104,D104,E104)</f>
+        <f t="shared" ref="F104:F111" si="4">SUM(C104,D104,E104)</f>
         <v>1800</v>
       </c>
     </row>
@@ -8010,7 +8240,7 @@
         <v>485</v>
       </c>
       <c r="F105">
-        <f>SUM(C105,D105,E105)</f>
+        <f t="shared" si="4"/>
         <v>1520</v>
       </c>
     </row>
@@ -8031,7 +8261,7 @@
         <v>450</v>
       </c>
       <c r="F106">
-        <f>SUM(C106,D106,E106)</f>
+        <f t="shared" si="4"/>
         <v>1510</v>
       </c>
     </row>
@@ -8052,7 +8282,7 @@
         <v>430</v>
       </c>
       <c r="F107">
-        <f>SUM(C107,D107,E107)</f>
+        <f t="shared" si="4"/>
         <v>1425</v>
       </c>
     </row>
@@ -8073,7 +8303,7 @@
         <v>420</v>
       </c>
       <c r="F108">
-        <f>SUM(C108,D108,E108)</f>
+        <f t="shared" si="4"/>
         <v>870</v>
       </c>
     </row>
@@ -8094,7 +8324,7 @@
         <v>410</v>
       </c>
       <c r="F109">
-        <f>SUM(C109,D109,E109)</f>
+        <f t="shared" si="4"/>
         <v>840</v>
       </c>
     </row>
@@ -8115,7 +8345,7 @@
         <v>550</v>
       </c>
       <c r="F110">
-        <f>SUM(C110,D110,E110)</f>
+        <f t="shared" si="4"/>
         <v>550</v>
       </c>
     </row>
@@ -8136,7 +8366,7 @@
         <v>510</v>
       </c>
       <c r="F111">
-        <f>SUM(C111,D111,E111)</f>
+        <f t="shared" si="4"/>
         <v>510</v>
       </c>
     </row>
@@ -8199,7 +8429,7 @@
         <v>550</v>
       </c>
       <c r="F119">
-        <f>SUM(C119,D119,E119)</f>
+        <f t="shared" ref="F119:F126" si="5">SUM(C119,D119,E119)</f>
         <v>1100</v>
       </c>
     </row>
@@ -8220,7 +8450,7 @@
         <v>510</v>
       </c>
       <c r="F120">
-        <f>SUM(C120,D120,E120)</f>
+        <f t="shared" si="5"/>
         <v>940</v>
       </c>
     </row>
@@ -8241,7 +8471,7 @@
         <v>0</v>
       </c>
       <c r="F121">
-        <f>SUM(C121,D121,E121)</f>
+        <f t="shared" si="5"/>
         <v>600</v>
       </c>
     </row>
@@ -8262,7 +8492,7 @@
         <v>600</v>
       </c>
       <c r="F122">
-        <f>SUM(C122,D122,E122)</f>
+        <f t="shared" si="5"/>
         <v>600</v>
       </c>
     </row>
@@ -8283,7 +8513,7 @@
         <v>0</v>
       </c>
       <c r="F123">
-        <f>SUM(C123,D123,E123)</f>
+        <f t="shared" si="5"/>
         <v>510</v>
       </c>
     </row>
@@ -8304,7 +8534,7 @@
         <v>0</v>
       </c>
       <c r="F124">
-        <f>SUM(C124,D124,E124)</f>
+        <f t="shared" si="5"/>
         <v>485</v>
       </c>
     </row>
@@ -8325,7 +8555,7 @@
         <v>0</v>
       </c>
       <c r="F125">
-        <f>SUM(C125,D125,E125)</f>
+        <f t="shared" si="5"/>
         <v>450</v>
       </c>
     </row>
@@ -8346,7 +8576,7 @@
         <v>0</v>
       </c>
       <c r="F126">
-        <f>SUM(C126,D126,E126)</f>
+        <f t="shared" si="5"/>
         <v>420</v>
       </c>
     </row>
@@ -8443,7 +8673,2058 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2A9064-8326-4D83-8C00-3ADDB8778C93}">
+  <dimension ref="A1:H118"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection sqref="A1:H118"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>8</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <v>9</v>
+      </c>
+      <c r="F28">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>11</v>
+      </c>
+      <c r="H28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>136</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
+      </c>
+      <c r="H29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>15</v>
+      </c>
+      <c r="H30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
+      </c>
+      <c r="E33">
+        <v>13</v>
+      </c>
+      <c r="G33">
+        <v>14</v>
+      </c>
+      <c r="H33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
+      </c>
+      <c r="E36">
+        <v>7</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="G36">
+        <v>7</v>
+      </c>
+      <c r="H36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37">
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <v>16</v>
+      </c>
+      <c r="F37">
+        <v>11</v>
+      </c>
+      <c r="G37">
+        <v>12</v>
+      </c>
+      <c r="H37">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>6</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+      <c r="D39">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>7</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>136</v>
+      </c>
+      <c r="F41">
+        <v>9</v>
+      </c>
+      <c r="G41">
+        <v>13</v>
+      </c>
+      <c r="H41">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>6</v>
+      </c>
+      <c r="G43">
+        <v>5</v>
+      </c>
+      <c r="H43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>168</v>
+      </c>
+      <c r="B47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47">
+        <v>11</v>
+      </c>
+      <c r="D47">
+        <v>11</v>
+      </c>
+      <c r="E47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>169</v>
+      </c>
+      <c r="B48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48">
+        <v>14</v>
+      </c>
+      <c r="D48">
+        <v>14</v>
+      </c>
+      <c r="E48">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" t="s">
+        <v>136</v>
+      </c>
+      <c r="G50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>143</v>
+      </c>
+      <c r="B55" t="s">
+        <v>142</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" t="s">
+        <v>142</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>170</v>
+      </c>
+      <c r="B57" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57" t="s">
+        <v>167</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+      <c r="H60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" t="s">
+        <v>145</v>
+      </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="G64">
+        <v>6</v>
+      </c>
+      <c r="H64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66" t="s">
+        <v>145</v>
+      </c>
+      <c r="C66">
+        <v>14</v>
+      </c>
+      <c r="D66">
+        <v>17</v>
+      </c>
+      <c r="E66">
+        <v>15</v>
+      </c>
+      <c r="F66">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>171</v>
+      </c>
+      <c r="B67" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67">
+        <v>13</v>
+      </c>
+      <c r="D67">
+        <v>13</v>
+      </c>
+      <c r="E67">
+        <v>13</v>
+      </c>
+      <c r="F67">
+        <v>12</v>
+      </c>
+      <c r="G67">
+        <v>11</v>
+      </c>
+      <c r="H67">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69" t="s">
+        <v>145</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>15</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>3</v>
+      </c>
+      <c r="G69">
+        <v>2</v>
+      </c>
+      <c r="H69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" t="s">
+        <v>145</v>
+      </c>
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+      <c r="E70">
+        <v>5</v>
+      </c>
+      <c r="F70">
+        <v>7</v>
+      </c>
+      <c r="G70">
+        <v>5</v>
+      </c>
+      <c r="H70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" t="s">
+        <v>145</v>
+      </c>
+      <c r="D71">
+        <v>16</v>
+      </c>
+      <c r="E71">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>145</v>
+      </c>
+      <c r="F73">
+        <v>4</v>
+      </c>
+      <c r="G73">
+        <v>12</v>
+      </c>
+      <c r="H73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>147</v>
+      </c>
+      <c r="B74" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74">
+        <v>12</v>
+      </c>
+      <c r="D74">
+        <v>10</v>
+      </c>
+      <c r="E74">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" t="s">
+        <v>145</v>
+      </c>
+      <c r="C76">
+        <v>10</v>
+      </c>
+      <c r="D76">
+        <v>12</v>
+      </c>
+      <c r="E76">
+        <v>6</v>
+      </c>
+      <c r="F76">
+        <v>11</v>
+      </c>
+      <c r="G76">
+        <v>9</v>
+      </c>
+      <c r="H76">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77" t="s">
+        <v>145</v>
+      </c>
+      <c r="C77">
+        <v>7</v>
+      </c>
+      <c r="D77">
+        <v>5</v>
+      </c>
+      <c r="E77">
+        <v>17</v>
+      </c>
+      <c r="F77">
+        <v>5</v>
+      </c>
+      <c r="G77">
+        <v>4</v>
+      </c>
+      <c r="H77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>149</v>
+      </c>
+      <c r="B78" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>104</v>
+      </c>
+      <c r="B79" t="s">
+        <v>145</v>
+      </c>
+      <c r="C79">
+        <v>9</v>
+      </c>
+      <c r="D79">
+        <v>7</v>
+      </c>
+      <c r="E79">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>150</v>
+      </c>
+      <c r="B80" t="s">
+        <v>145</v>
+      </c>
+      <c r="C80">
+        <v>6</v>
+      </c>
+      <c r="D80">
+        <v>14</v>
+      </c>
+      <c r="F80">
+        <v>8</v>
+      </c>
+      <c r="G80">
+        <v>10</v>
+      </c>
+      <c r="H80">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" t="s">
+        <v>145</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>6</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" t="s">
+        <v>145</v>
+      </c>
+      <c r="D82">
+        <v>8</v>
+      </c>
+      <c r="E82">
+        <v>8</v>
+      </c>
+      <c r="F82">
+        <v>10</v>
+      </c>
+      <c r="G82">
+        <v>8</v>
+      </c>
+      <c r="H82">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>37</v>
+      </c>
+      <c r="B83" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>151</v>
+      </c>
+      <c r="B84" t="s">
+        <v>145</v>
+      </c>
+      <c r="F84">
+        <v>9</v>
+      </c>
+      <c r="G84">
+        <v>7</v>
+      </c>
+      <c r="H84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" t="s">
+        <v>145</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+      <c r="E85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" t="s">
+        <v>145</v>
+      </c>
+      <c r="C86">
+        <v>8</v>
+      </c>
+      <c r="D86">
+        <v>6</v>
+      </c>
+      <c r="E86">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" t="s">
+        <v>145</v>
+      </c>
+      <c r="C87">
+        <v>11</v>
+      </c>
+      <c r="D87">
+        <v>9</v>
+      </c>
+      <c r="E87">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" t="s">
+        <v>145</v>
+      </c>
+      <c r="D88">
+        <v>11</v>
+      </c>
+      <c r="E88">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>59</v>
+      </c>
+      <c r="B90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>110</v>
+      </c>
+      <c r="B91" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+      <c r="D91">
+        <v>16</v>
+      </c>
+      <c r="E91">
+        <v>3</v>
+      </c>
+      <c r="F91">
+        <v>14</v>
+      </c>
+      <c r="G91">
+        <v>4</v>
+      </c>
+      <c r="H91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>152</v>
+      </c>
+      <c r="B92" t="s">
+        <v>10</v>
+      </c>
+      <c r="F92">
+        <v>12</v>
+      </c>
+      <c r="G92">
+        <v>9</v>
+      </c>
+      <c r="H92">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>84</v>
+      </c>
+      <c r="B94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>15</v>
+      </c>
+      <c r="B95" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95">
+        <v>8</v>
+      </c>
+      <c r="D95">
+        <v>9</v>
+      </c>
+      <c r="E95">
+        <v>8</v>
+      </c>
+      <c r="F95">
+        <v>8</v>
+      </c>
+      <c r="G95">
+        <v>6</v>
+      </c>
+      <c r="H95">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>19</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96">
+        <v>7</v>
+      </c>
+      <c r="D96">
+        <v>7</v>
+      </c>
+      <c r="E96">
+        <v>12</v>
+      </c>
+      <c r="F96">
+        <v>7</v>
+      </c>
+      <c r="G96">
+        <v>12</v>
+      </c>
+      <c r="H96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>153</v>
+      </c>
+      <c r="B97" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97">
+        <v>9</v>
+      </c>
+      <c r="G97">
+        <v>10</v>
+      </c>
+      <c r="H97">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>154</v>
+      </c>
+      <c r="B98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>155</v>
+      </c>
+      <c r="B99" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>112</v>
+      </c>
+      <c r="B100" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100">
+        <v>15</v>
+      </c>
+      <c r="D100">
+        <v>10</v>
+      </c>
+      <c r="F100">
+        <v>6</v>
+      </c>
+      <c r="G100">
+        <v>11</v>
+      </c>
+      <c r="H100">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>156</v>
+      </c>
+      <c r="B101" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <v>4</v>
+      </c>
+      <c r="D101">
+        <v>4</v>
+      </c>
+      <c r="E101">
+        <v>7</v>
+      </c>
+      <c r="F101">
+        <v>5</v>
+      </c>
+      <c r="H101">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" t="s">
+        <v>10</v>
+      </c>
+      <c r="F102">
+        <v>4</v>
+      </c>
+      <c r="G102">
+        <v>5</v>
+      </c>
+      <c r="H102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>157</v>
+      </c>
+      <c r="B103" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>158</v>
+      </c>
+      <c r="B104" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>159</v>
+      </c>
+      <c r="B105" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>9</v>
+      </c>
+      <c r="E105">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>160</v>
+      </c>
+      <c r="B106" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106">
+        <v>10</v>
+      </c>
+      <c r="D106">
+        <v>6</v>
+      </c>
+      <c r="E106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107" t="s">
+        <v>10</v>
+      </c>
+      <c r="C107">
+        <v>5</v>
+      </c>
+      <c r="D107">
+        <v>3</v>
+      </c>
+      <c r="E107">
+        <v>15</v>
+      </c>
+      <c r="F107">
+        <v>2</v>
+      </c>
+      <c r="G107">
+        <v>3</v>
+      </c>
+      <c r="H107">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>173</v>
+      </c>
+      <c r="B108" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108">
+        <v>2</v>
+      </c>
+      <c r="E108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>16</v>
+      </c>
+      <c r="B109" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109">
+        <v>6</v>
+      </c>
+      <c r="D109">
+        <v>8</v>
+      </c>
+      <c r="E109">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>99</v>
+      </c>
+      <c r="B110" t="s">
+        <v>10</v>
+      </c>
+      <c r="C110">
+        <v>11</v>
+      </c>
+      <c r="E110">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>174</v>
+      </c>
+      <c r="B111" t="s">
+        <v>10</v>
+      </c>
+      <c r="C111">
+        <v>12</v>
+      </c>
+      <c r="D111">
+        <v>12</v>
+      </c>
+      <c r="E111">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>175</v>
+      </c>
+      <c r="B112" t="s">
+        <v>10</v>
+      </c>
+      <c r="C112">
+        <v>14</v>
+      </c>
+      <c r="D112">
+        <v>13</v>
+      </c>
+      <c r="E112">
+        <v>11</v>
+      </c>
+      <c r="F112">
+        <v>10</v>
+      </c>
+      <c r="H112">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>176</v>
+      </c>
+      <c r="B113" t="s">
+        <v>10</v>
+      </c>
+      <c r="C113">
+        <v>16</v>
+      </c>
+      <c r="D113">
+        <v>14</v>
+      </c>
+      <c r="E113">
+        <v>13</v>
+      </c>
+      <c r="F113">
+        <v>13</v>
+      </c>
+      <c r="G113">
+        <v>7</v>
+      </c>
+      <c r="H113">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>63</v>
+      </c>
+      <c r="B114" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114">
+        <v>17</v>
+      </c>
+      <c r="D114">
+        <v>15</v>
+      </c>
+      <c r="E114">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>177</v>
+      </c>
+      <c r="B115" t="s">
+        <v>10</v>
+      </c>
+      <c r="C115">
+        <v>18</v>
+      </c>
+      <c r="D115">
+        <v>11</v>
+      </c>
+      <c r="E115">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>57</v>
+      </c>
+      <c r="B116" t="s">
+        <v>10</v>
+      </c>
+      <c r="D116">
+        <v>5</v>
+      </c>
+      <c r="E116">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>179</v>
+      </c>
+      <c r="B117" t="s">
+        <v>10</v>
+      </c>
+      <c r="F117">
+        <v>3</v>
+      </c>
+      <c r="G117">
+        <v>2</v>
+      </c>
+      <c r="H117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>180</v>
+      </c>
+      <c r="B118" t="s">
+        <v>10</v>
+      </c>
+      <c r="F118">
+        <v>11</v>
+      </c>
+      <c r="G118">
+        <v>8</v>
+      </c>
+      <c r="H118">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6AF795D8A01FF43A9E4AF9E30B144DB" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ff7acb529109b266cdfa94bf47f11ec">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1346f0d-2271-46d3-b9c8-3d8c72d47be9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845eecb48e3f5109706bc8393ea6c74" ns3:_="">
     <xsd:import namespace="a1346f0d-2271-46d3-b9c8-3d8c72d47be9"/>
@@ -8575,22 +10856,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8972A39A-C6AE-440C-A903-BE881E6D34A2}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FD5D83C-D53F-4CBB-B688-480C957B700B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3D20D34-01E6-4F63-B80D-EF1EFB6E6003}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8606,18 +10886,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FD5D83C-D53F-4CBB-B688-480C957B700B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8972A39A-C6AE-440C-A903-BE881E6D34A2}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
 </file>
</xml_diff>